<commit_message>
v5 BOM and new back plate design
</commit_message>
<xml_diff>
--- a/kicad/seeed_production_files/ClockIOT_PCB/ClockIOT_PCB_specification.xlsx
+++ b/kicad/seeed_production_files/ClockIOT_PCB/ClockIOT_PCB_specification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,7 +46,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ClockIOT rev 4</t>
+    <t xml:space="preserve">ClockIOT rev 5</t>
   </si>
   <si>
     <r>
@@ -931,12 +931,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1008,20 +1008,20 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.1902834008097"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.5384615384615"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.54251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.336032388664"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.8825910931174"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="12.6842105263158"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="30.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="12.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1253,7 +1253,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1268,23 +1268,22 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11.90234375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="16" width="23.7368421052632"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="16" width="28.7935222672065"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="26.8218623481781"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.2226720647773"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.9109311740891"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="37.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="16" width="23.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="16" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="16" width="28.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="16" width="26.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1544,7 +1543,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>